<commit_message>
correcting case study headers
</commit_message>
<xml_diff>
--- a/pareto/models_extra/CM_module/case_studies/CM_large_permian.xlsx
+++ b/pareto/models_extra/CM_module/case_studies/CM_large_permian.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arshb11/main/Grad_Research/CM/project-pareto/pareto/case_studies/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arshb11/main/Grad_Research/CM/project-pareto/pareto/models_extra/CM_module/case_studies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98797434-9313-C348-ABDA-34D85CDFBBDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D2C2DE-52E2-394D-A929-1457A880F4E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" tabRatio="834" firstSheet="51" activeTab="60" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="3480" yWindow="2040" windowWidth="30240" windowHeight="17620" tabRatio="834" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -77,6 +77,7 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId62"/>
+    <externalReference r:id="rId63"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1858,6 +1859,209 @@
 </externalLink>
 </file>
 
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Overview"/>
+      <sheetName val="Schematic"/>
+      <sheetName val="Units"/>
+      <sheetName val="ProductionPads"/>
+      <sheetName val="ProductionTanks"/>
+      <sheetName val="CompletionsPads"/>
+      <sheetName val="SWDSites"/>
+      <sheetName val="WaterQualityComponents"/>
+      <sheetName val="FreshwaterSources"/>
+      <sheetName val="StorageSites"/>
+      <sheetName val="TreatmentSites"/>
+      <sheetName val="NetworkNodes"/>
+      <sheetName val="PNA"/>
+      <sheetName val="CNA"/>
+      <sheetName val="CCA"/>
+      <sheetName val="NNA"/>
+      <sheetName val="NCA"/>
+      <sheetName val="NKA"/>
+      <sheetName val="NRA"/>
+      <sheetName val="NSA"/>
+      <sheetName val="SNA"/>
+      <sheetName val="FCA"/>
+      <sheetName val="FNA"/>
+      <sheetName val="RCA"/>
+      <sheetName val="RSA"/>
+      <sheetName val="SCA"/>
+      <sheetName val="RNA"/>
+      <sheetName val="PCT"/>
+      <sheetName val="FCT"/>
+      <sheetName val="PKT"/>
+      <sheetName val="CKT"/>
+      <sheetName val="CCT"/>
+      <sheetName val="CST"/>
+      <sheetName val="CompletionsDemand"/>
+      <sheetName val="PadRates"/>
+      <sheetName val="FlowbackRates"/>
+      <sheetName val="InitialStorageLevel"/>
+      <sheetName val="InitialPipelineCapacity"/>
+      <sheetName val="InitialDisposalCapacity"/>
+      <sheetName val="InitialStorageCapacity"/>
+      <sheetName val="InitialTreatmentCapacity"/>
+      <sheetName val="FreshwaterSourcingAvailability"/>
+      <sheetName val="DisposalOperationalCost"/>
+      <sheetName val="TreatmentOperationalCost"/>
+      <sheetName val="PipelineOperationalCost"/>
+      <sheetName val="StorageCost"/>
+      <sheetName val="StorageWithdrawalRevenue"/>
+      <sheetName val="FreshSourcingCost"/>
+      <sheetName val="BeneficialReuseCost"/>
+      <sheetName val="BeneficialReuseRevenue"/>
+      <sheetName val="TruckingHourlyCost"/>
+      <sheetName val="TruckingTime"/>
+      <sheetName val="TreatmentEfficiency"/>
+      <sheetName val="RemovalEfficiency"/>
+      <sheetName val="DesalinationTechnologies"/>
+      <sheetName val="DesalinationSites"/>
+      <sheetName val="PadWaterQuality"/>
+      <sheetName val="StorageInitialWaterQuality"/>
+      <sheetName val="MinTreatmentFlow"/>
+      <sheetName val="MinResidualQuality"/>
+      <sheetName val="ComponentPrice"/>
+      <sheetName val="ComponentTreatment"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2">
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>INDEX</v>
+          </cell>
+          <cell r="B2" t="str">
+            <v>VALUE</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>volume</v>
+          </cell>
+          <cell r="B3" t="str">
+            <v>kbbl</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>distance</v>
+          </cell>
+          <cell r="B4" t="str">
+            <v>mile</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>diameter</v>
+          </cell>
+          <cell r="B5" t="str">
+            <v>inch</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>concentration</v>
+          </cell>
+          <cell r="B6" t="str">
+            <v>mg/liter</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>currency</v>
+          </cell>
+          <cell r="B7" t="str">
+            <v>USD</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>time</v>
+          </cell>
+          <cell r="B8" t="str">
+            <v>day</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>decision period</v>
+          </cell>
+          <cell r="B9" t="str">
+            <v>week</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="32" refreshError="1"/>
+      <sheetData sheetId="33" refreshError="1"/>
+      <sheetData sheetId="34" refreshError="1"/>
+      <sheetData sheetId="35" refreshError="1"/>
+      <sheetData sheetId="36" refreshError="1"/>
+      <sheetData sheetId="37" refreshError="1"/>
+      <sheetData sheetId="38" refreshError="1"/>
+      <sheetData sheetId="39" refreshError="1"/>
+      <sheetData sheetId="40" refreshError="1"/>
+      <sheetData sheetId="41" refreshError="1"/>
+      <sheetData sheetId="42" refreshError="1"/>
+      <sheetData sheetId="43" refreshError="1"/>
+      <sheetData sheetId="44" refreshError="1"/>
+      <sheetData sheetId="45" refreshError="1"/>
+      <sheetData sheetId="46" refreshError="1"/>
+      <sheetData sheetId="47" refreshError="1"/>
+      <sheetData sheetId="48" refreshError="1"/>
+      <sheetData sheetId="49" refreshError="1"/>
+      <sheetData sheetId="50" refreshError="1"/>
+      <sheetData sheetId="51" refreshError="1"/>
+      <sheetData sheetId="52" refreshError="1"/>
+      <sheetData sheetId="53" refreshError="1"/>
+      <sheetData sheetId="54" refreshError="1"/>
+      <sheetData sheetId="55" refreshError="1"/>
+      <sheetData sheetId="56" refreshError="1"/>
+      <sheetData sheetId="57" refreshError="1"/>
+      <sheetData sheetId="58" refreshError="1"/>
+      <sheetData sheetId="59" refreshError="1"/>
+      <sheetData sheetId="60" refreshError="1"/>
+      <sheetData sheetId="61" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -2160,7 +2364,7 @@
   </sheetPr>
   <dimension ref="B1:M37"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6691,7 +6895,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7651,8 +7855,8 @@
   </sheetPr>
   <dimension ref="A1:BD10"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView showZeros="0" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7667,9 +7871,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:56" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="e">
-        <f>_xlfn.CONCAT( "Table of Completions Water Demand for Completions Sites over ",VLOOKUP("decision period",#REF!, 2, FALSE),"s [",VLOOKUP("volume",#REF!, 2, FALSE),"/", VLOOKUP("time",#REF!, 2, FALSE),"]")</f>
-        <v>#REF!</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Completions Water Demand for Completions Sites over ",VLOOKUP("decision period", [2]Units!$A$2:$B$9, 2, FALSE),"s [",VLOOKUP("volume", [2]Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", [2]Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Completions Water Demand for Completions Sites over weeks [kbbl/day]</v>
       </c>
     </row>
     <row r="2" spans="1:56" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -8344,7 +8548,7 @@
   </sheetPr>
   <dimension ref="A1:BA20"/>
   <sheetViews>
-    <sheetView topLeftCell="AN1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8356,9 +8560,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="e">
-        <f>_xlfn.CONCAT( "Table of Production Rate Forecasts by Pads [",VLOOKUP("volume",#REF!, 2, FALSE),"/", VLOOKUP("time",#REF!, 2, FALSE),"]")</f>
-        <v>#REF!</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Production Rate Forecasts by Pads [",VLOOKUP("volume", [2]Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", [2]Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Production Rate Forecasts by Pads [kbbl/day]</v>
       </c>
     </row>
     <row r="2" spans="1:53" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -11527,9 +11731,7 @@
   </sheetPr>
   <dimension ref="A1:BA8"/>
   <sheetViews>
-    <sheetView topLeftCell="AK1" workbookViewId="0">
-      <selection activeCell="BB10" sqref="BB10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11542,9 +11744,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="e">
-        <f>_xlfn.CONCAT( "Table of Flowback Rate Forecasts by Pads [",VLOOKUP("volume",#REF!, 2, FALSE),"/", VLOOKUP("time",#REF!, 2, FALSE),"]")</f>
-        <v>#REF!</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Flowback Rate Forecasts by Pads [",VLOOKUP("volume", [2]Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", [2]Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Flowback Rate Forecasts by Pads [kbbl/day]</v>
       </c>
     </row>
     <row r="2" spans="1:53" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -12316,9 +12518,7 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12327,9 +12527,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="e">
-        <f>_xlfn.CONCAT( "Table of Initial Storage Capacity [",VLOOKUP("volume",#REF!, 2, FALSE),"]")</f>
-        <v>#REF!</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Initial Storage Capacity [",VLOOKUP("volume", [2]Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Initial Storage Capacity [kbbl]</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -12377,9 +12577,7 @@
   </sheetPr>
   <dimension ref="A1:AR56"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="T1" zoomScale="125" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="V29" sqref="V29"/>
-    </sheetView>
+    <sheetView showZeros="0" zoomScale="125" zoomScaleNormal="60" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12387,9 +12585,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="e">
-        <f>_xlfn.CONCAT( "Table of Initial Pipeline Capacity between Sites [",VLOOKUP("volume",#REF!, 2, FALSE),"/", VLOOKUP("time",#REF!, 2, FALSE),"]")</f>
-        <v>#REF!</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Initial Pipeline Capacity between Sites [",VLOOKUP("volume", [2]Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", [2]Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Initial Pipeline Capacity between Sites [kbbl/day]</v>
       </c>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.2">
@@ -19773,9 +19971,7 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -19784,9 +19980,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="e">
-        <f>_xlfn.CONCAT( "Table of Initial Disposal Capacity [",VLOOKUP("volume",#REF!, 2, FALSE),"/", VLOOKUP("time",#REF!, 2, FALSE),"]")</f>
-        <v>#REF!</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Initial Disposal Capacity [",VLOOKUP("volume", [2]Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", [2]Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Initial Disposal Capacity [kbbl/day]</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -19957,9 +20153,7 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -19969,9 +20163,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="e">
-        <f>_xlfn.CONCAT( "Table of Initial Treatment Capacity [",VLOOKUP("volume",#REF!, 2, FALSE),"/", VLOOKUP("time",#REF!, 2, FALSE),"]")</f>
-        <v>#REF!</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Initial Treatment Capacity [",VLOOKUP("volume", [2]Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", [2]Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Initial Treatment Capacity [kbbl/day]</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -20027,9 +20221,7 @@
   </sheetPr>
   <dimension ref="A1:BA15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -20038,9 +20230,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="e">
-        <f>_xlfn.CONCAT( "Table of Freshwater Sourcing Availability [",VLOOKUP("volume",#REF!, 2, FALSE),"/", VLOOKUP("time",#REF!, 2, FALSE),"]")</f>
-        <v>#REF!</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Freshwater Sourcing Availability [",VLOOKUP("volume", [2]Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", [2]Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Freshwater Sourcing Availability [kbbl/day]</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>86</v>
@@ -20674,9 +20866,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="e">
-        <f>_xlfn.CONCAT( "Table of Disposal Operational Cost [",VLOOKUP("currency",#REF!, 2, FALSE),"/", VLOOKUP("volume",#REF!, 2, FALSE),"]")</f>
-        <v>#REF!</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Disposal Operational Cost [",VLOOKUP("currency", [2]Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", [2]Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Disposal Operational Cost [USD/kbbl]</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -20741,9 +20933,7 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -20752,9 +20942,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="e">
-        <f>_xlfn.CONCAT( "Table of Treatment Operational Cost [",VLOOKUP("currency",#REF!, 2, FALSE),"/", VLOOKUP("volume",#REF!, 2, FALSE),"]")</f>
-        <v>#REF!</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Treatment Operational Cost [",VLOOKUP("currency", [2]Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", [2]Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Treatment Operational Cost [USD/kbbl]</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -20811,8 +21001,8 @@
   </sheetPr>
   <dimension ref="A1:AR56"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" zoomScale="88" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AF31" sqref="AF31"/>
+    <sheetView zoomScale="88" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20823,9 +21013,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="e">
-        <f>_xlfn.CONCAT( "Table of Pipeline Operational Cost between Sites [",VLOOKUP("currency",#REF!, 2, FALSE),"/", VLOOKUP("volume",#REF!, 2, FALSE),"]")</f>
-        <v>#REF!</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Pipeline Operational Cost between Sites [",VLOOKUP("currency", [2]Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", [2]Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Pipeline Operational Cost between Sites [USD/kbbl]</v>
       </c>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.2">
@@ -28329,9 +28519,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="e">
-        <f>_xlfn.CONCAT( "Table of Freshwater Souring Cost [",VLOOKUP("currency",#REF!, 2, FALSE),"/", VLOOKUP("volume",#REF!, 2, FALSE),"]")</f>
-        <v>#REF!</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Freshwater Souring Cost [",VLOOKUP("currency", [2]Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", [2]Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Freshwater Souring Cost [USD/kbbl]</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -28553,7 +28743,9 @@
   </sheetPr>
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -28561,9 +28753,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="e">
-        <f>_xlfn.CONCAT( "Table of Trucking Hourly Cost [",VLOOKUP("currency",#REF!, 2, FALSE),"/", "hour","]")</f>
-        <v>#REF!</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Trucking Hourly Cost [",VLOOKUP("currency", [2]Units!$A$2:$B$9, 2, FALSE),"/", "hour","]")</f>
+        <v>Table of Trucking Hourly Cost [USD/hour]</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -29883,7 +30075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E02D577-3E8C-444E-87B2-8DF0DDD275D2}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>

</xml_diff>